<commit_message>
Aggiunte le prime tabelle degli accessi
</commit_message>
<xml_diff>
--- a/Relazione/Tabelle/TabellaFrequenze.xlsx
+++ b/Relazione/Tabelle/TabellaFrequenze.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\Basi_Di_Dati_2021\Relazione\Tabelle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44753F8D-7C52-446C-975A-BCB1EA54A2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C7369-5596-407F-AF38-4D1BA4E915C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{AD9BB531-DC17-450C-91DA-063E7B2B509D}"/>
+    <workbookView xWindow="13813" yWindow="1273" windowWidth="9600" windowHeight="6000" xr2:uid="{AD9BB531-DC17-450C-91DA-063E7B2B509D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Iniziare un impianto elettrico per un cliente</t>
   </si>
   <si>
-    <t>Aggiornare i materiali in magazzino</t>
-  </si>
-  <si>
     <t>Registrare il turno lavorativo</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>1 al mese</t>
+  </si>
+  <si>
+    <t>Aggiornare le quantità dei materiali in magazzino</t>
   </si>
 </sst>
 </file>
@@ -120,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,12 +139,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -265,18 +259,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -595,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFBC3188-8127-439C-8C36-101E3C50DAF9}">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -624,10 +618,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.5">
@@ -638,7 +632,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.5">
@@ -649,7 +643,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.5">
@@ -657,10 +651,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.5">
@@ -668,10 +662,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.5">
@@ -679,10 +673,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.5">
@@ -690,10 +684,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.5">
@@ -701,10 +695,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.5">
@@ -712,10 +706,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.5">
@@ -723,10 +717,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminata le tabelle degli accessi
</commit_message>
<xml_diff>
--- a/Relazione/Tabelle/TabellaFrequenze.xlsx
+++ b/Relazione/Tabelle/TabellaFrequenze.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\Basi_Di_Dati_2021\Relazione\Tabelle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C7369-5596-407F-AF38-4D1BA4E915C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C69A629-BA44-4474-BC03-2677B6F88C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13813" yWindow="1273" windowWidth="9600" windowHeight="6000" xr2:uid="{AD9BB531-DC17-450C-91DA-063E7B2B509D}"/>
+    <workbookView xWindow="20660" yWindow="11200" windowWidth="9600" windowHeight="6000" xr2:uid="{AD9BB531-DC17-450C-91DA-063E7B2B509D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Numero</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Inserire un nuovo cliente</t>
   </si>
   <si>
-    <t>Contare le ore lavorative degli elettricisti nell'ultimo mese</t>
-  </si>
-  <si>
     <t>5 al mese</t>
   </si>
   <si>
@@ -81,22 +78,28 @@
     <t>3 al mese</t>
   </si>
   <si>
-    <t>10 al giorno</t>
-  </si>
-  <si>
     <t>20 al giorno</t>
   </si>
   <si>
-    <t>4 al giorno</t>
-  </si>
-  <si>
     <t>10 al mese</t>
   </si>
   <si>
-    <t>1 al mese</t>
-  </si>
-  <si>
     <t>Aggiornare le quantità dei materiali in magazzino</t>
+  </si>
+  <si>
+    <t>Inserire un nuovo elettricista</t>
+  </si>
+  <si>
+    <t>1 all'anno</t>
+  </si>
+  <si>
+    <t>25 al giorno</t>
+  </si>
+  <si>
+    <t>2 al giorno</t>
+  </si>
+  <si>
+    <t>Contare le ore lavorative di un elettricista nell'ultimo mese</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -201,37 +204,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -266,13 +238,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -587,19 +559,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFBC3188-8127-439C-8C36-101E3C50DAF9}">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="46.5859375" customWidth="1"/>
+    <col min="3" max="3" width="47.3515625" customWidth="1"/>
     <col min="4" max="4" width="11.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -610,10 +582,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.5">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -621,10 +593,10 @@
         <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B5" s="8">
         <v>2</v>
       </c>
@@ -632,10 +604,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -643,21 +615,21 @@
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B7" s="8">
         <v>4</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -665,10 +637,11 @@
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B9" s="8">
         <v>6</v>
       </c>
@@ -676,51 +649,62 @@
         <v>6</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>7</v>
+      <c r="C10" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B11" s="8">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>8</v>
+      <c r="C11" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.5">
       <c r="B12" s="5">
         <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B13" s="8">
+        <v>10</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B13" s="11">
-        <v>10</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="D13" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B14" s="5">
         <v>11</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>19</v>
+      <c r="C14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>